<commit_message>
update config for deployment
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Thaiairways/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Thaiairways/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Thaiairways\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F090D970-FFED-4E01-A4EE-9F4DB1BB0356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A23DC66-947F-4CD1-BAD3-BF49F6BD5571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="1932" windowWidth="21588" windowHeight="10644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -181,9 +181,6 @@
     <t>PathSAKey</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_UploadBucket</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -193,37 +190,40 @@
     <t>DialogDownloadChrome</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathDownloadChrome</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_DialogDownloadChrome</t>
-  </si>
-  <si>
     <t>SenderName</t>
   </si>
   <si>
     <t>RPA_Moon_SenderName</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
-  </si>
-  <si>
     <t>RPA206_ThaiAirways_RefID</t>
   </si>
   <si>
     <t>RefId</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_Cred_Gmail</t>
+    <t>RPA_Moon_SheetIdConfig_Transport</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA_Moon_DialogDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
+    <t>RPA_Moon_Cred_Gmail</t>
   </si>
 </sst>
 </file>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -650,10 +650,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -1693,7 +1693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2912,7 +2912,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -2920,7 +2920,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -2928,7 +2928,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -2936,39 +2936,39 @@
         <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>